<commit_message>
add images fix bug v1
</commit_message>
<xml_diff>
--- a/Offre.xlsx
+++ b/Offre.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>title</t>
   </si>
@@ -26,31 +26,40 @@
     <t>provider</t>
   </si>
   <si>
-    <t>mohsen</t>
+    <t>Work-Study</t>
   </si>
   <si>
-    <t>lll</t>
+    <t>Work-Study opportunity come and check this out and don't waste this</t>
   </si>
   <si>
     <t>Alternance</t>
   </si>
   <si>
+    <t xml:space="preserve">sofrecom </t>
+  </si>
+  <si>
+    <t>mobile dev internship</t>
+  </si>
+  <si>
+    <t>We are offering mobile development internship</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Stage d'été</t>
+  </si>
+  <si>
+    <t>Étudiant(e) à la recherche d'un stage d'été ?</t>
+  </si>
+  <si>
     <t>Vermeg</t>
   </si>
   <si>
-    <t>tttttttttttttt</t>
+    <t>Alternance 2022</t>
   </si>
   <si>
-    <t>tttttttttttttttttt</t>
-  </si>
-  <si>
-    <t>bbbbbbbb</t>
-  </si>
-  <si>
-    <t>bbbbbbb</t>
-  </si>
-  <si>
-    <t>Stage</t>
+    <t>Étudiant(e) à la recherche d'un alternance ?</t>
   </si>
 </sst>
 </file>
@@ -102,14 +111,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.35546875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="14.39453125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="20.546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="63.67578125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="11.43359375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.265625" customWidth="true" bestFit="true"/>
   </cols>
@@ -144,13 +153,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -158,100 +167,30 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>